<commit_message>
Ejercicio finalizado. Añadido el control de nombres de proyecto.
</commit_message>
<xml_diff>
--- a/proyectos.xlsx
+++ b/proyectos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q05432593\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S28937764\Documents\EjercicioFebrero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E345D0-1A42-4DAB-87A7-572B429D4A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7E5B96-FF96-460F-A6DF-D3E228F54D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F3929C5C-5F02-4ABB-BB12-326D8E50090B}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="8685" xr2:uid="{F3929C5C-5F02-4ABB-BB12-326D8E50090B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
   <si>
     <t>AL258112</t>
   </si>
@@ -207,6 +207,33 @@
   </si>
   <si>
     <t>UR047451</t>
+  </si>
+  <si>
+    <t>UL2581221</t>
+  </si>
+  <si>
+    <t>Control System Development</t>
+  </si>
+  <si>
+    <t>Testing control method</t>
+  </si>
+  <si>
+    <t>UL2581999</t>
+  </si>
+  <si>
+    <t>1L258199</t>
+  </si>
+  <si>
+    <t>U1258199</t>
+  </si>
+  <si>
+    <t>ULA58199</t>
+  </si>
+  <si>
+    <t>UL2A8199</t>
+  </si>
+  <si>
+    <t>UL25819A</t>
   </si>
 </sst>
 </file>
@@ -228,12 +255,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -248,8 +281,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,7 +590,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -564,9 +598,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8167FEE-14CF-4C1D-9C2E-AED5800257E1}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -940,6 +976,92 @@
         <v>8</v>
       </c>
     </row>
+    <row r="27" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>